<commit_message>
real ip modify & grade init
</commit_message>
<xml_diff>
--- a/data/real_ip.xlsx
+++ b/data/real_ip.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="721">
   <si>
     <t>10.96.121.1</t>
   </si>
@@ -745,6 +745,1454 @@
   <si>
     <t>hakbun</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.122.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.122.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.122.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.122.5</t>
+  </si>
+  <si>
+    <t>10.96.122.7</t>
+  </si>
+  <si>
+    <t>10.96.122.9</t>
+  </si>
+  <si>
+    <t>10.96.122.11</t>
+  </si>
+  <si>
+    <t>10.96.122.13</t>
+  </si>
+  <si>
+    <t>10.96.122.15</t>
+  </si>
+  <si>
+    <t>10.96.122.17</t>
+  </si>
+  <si>
+    <t>10.96.122.19</t>
+  </si>
+  <si>
+    <t>10.96.122.21</t>
+  </si>
+  <si>
+    <t>10.96.122.23</t>
+  </si>
+  <si>
+    <t>10.96.122.25</t>
+  </si>
+  <si>
+    <t>10.96.122.27</t>
+  </si>
+  <si>
+    <t>10.96.122.29</t>
+  </si>
+  <si>
+    <t>10.96.122.31</t>
+  </si>
+  <si>
+    <t>10.96.122.33</t>
+  </si>
+  <si>
+    <t>10.96.122.35</t>
+  </si>
+  <si>
+    <t>10.96.122.37</t>
+  </si>
+  <si>
+    <t>10.96.122.39</t>
+  </si>
+  <si>
+    <t>10.96.122.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.122.6</t>
+  </si>
+  <si>
+    <t>10.96.122.8</t>
+  </si>
+  <si>
+    <t>10.96.122.10</t>
+  </si>
+  <si>
+    <t>10.96.122.12</t>
+  </si>
+  <si>
+    <t>10.96.122.14</t>
+  </si>
+  <si>
+    <t>10.96.122.16</t>
+  </si>
+  <si>
+    <t>10.96.122.18</t>
+  </si>
+  <si>
+    <t>10.96.122.20</t>
+  </si>
+  <si>
+    <t>10.96.122.22</t>
+  </si>
+  <si>
+    <t>10.96.122.24</t>
+  </si>
+  <si>
+    <t>10.96.122.26</t>
+  </si>
+  <si>
+    <t>10.96.122.28</t>
+  </si>
+  <si>
+    <t>10.96.122.30</t>
+  </si>
+  <si>
+    <t>10.96.122.32</t>
+  </si>
+  <si>
+    <t>10.96.122.34</t>
+  </si>
+  <si>
+    <t>10.96.122.36</t>
+  </si>
+  <si>
+    <t>10.96.122.38</t>
+  </si>
+  <si>
+    <t>10.96.122.40</t>
+  </si>
+  <si>
+    <t>10.96.122.41</t>
+  </si>
+  <si>
+    <t>10.96.122.43</t>
+  </si>
+  <si>
+    <t>10.96.122.45</t>
+  </si>
+  <si>
+    <t>10.96.122.47</t>
+  </si>
+  <si>
+    <t>10.96.122.49</t>
+  </si>
+  <si>
+    <t>10.96.122.51</t>
+  </si>
+  <si>
+    <t>10.96.122.53</t>
+  </si>
+  <si>
+    <t>10.96.122.55</t>
+  </si>
+  <si>
+    <t>10.96.122.57</t>
+  </si>
+  <si>
+    <t>10.96.122.59</t>
+  </si>
+  <si>
+    <t>10.96.122.61</t>
+  </si>
+  <si>
+    <t>10.96.122.63</t>
+  </si>
+  <si>
+    <t>10.96.122.65</t>
+  </si>
+  <si>
+    <t>10.96.122.67</t>
+  </si>
+  <si>
+    <t>10.96.122.69</t>
+  </si>
+  <si>
+    <t>10.96.122.71</t>
+  </si>
+  <si>
+    <t>10.96.122.73</t>
+  </si>
+  <si>
+    <t>10.96.122.75</t>
+  </si>
+  <si>
+    <t>10.96.122.77</t>
+  </si>
+  <si>
+    <t>10.96.122.79</t>
+  </si>
+  <si>
+    <t>10.96.122.42</t>
+  </si>
+  <si>
+    <t>10.96.122.44</t>
+  </si>
+  <si>
+    <t>10.96.122.46</t>
+  </si>
+  <si>
+    <t>10.96.122.48</t>
+  </si>
+  <si>
+    <t>10.96.122.50</t>
+  </si>
+  <si>
+    <t>10.96.122.52</t>
+  </si>
+  <si>
+    <t>10.96.122.54</t>
+  </si>
+  <si>
+    <t>10.96.122.56</t>
+  </si>
+  <si>
+    <t>10.96.122.58</t>
+  </si>
+  <si>
+    <t>10.96.122.60</t>
+  </si>
+  <si>
+    <t>10.96.122.62</t>
+  </si>
+  <si>
+    <t>10.96.122.64</t>
+  </si>
+  <si>
+    <t>10.96.122.66</t>
+  </si>
+  <si>
+    <t>10.96.122.68</t>
+  </si>
+  <si>
+    <t>10.96.122.70</t>
+  </si>
+  <si>
+    <t>10.96.122.72</t>
+  </si>
+  <si>
+    <t>10.96.122.74</t>
+  </si>
+  <si>
+    <t>10.96.122.76</t>
+  </si>
+  <si>
+    <t>10.96.122.78</t>
+  </si>
+  <si>
+    <t>10.96.122.80</t>
+  </si>
+  <si>
+    <t>10.96.122.81</t>
+  </si>
+  <si>
+    <t>10.96.122.82</t>
+  </si>
+  <si>
+    <t>10.96.122.83</t>
+  </si>
+  <si>
+    <t>10.96.122.84</t>
+  </si>
+  <si>
+    <t>10.96.122.85</t>
+  </si>
+  <si>
+    <t>10.96.122.86</t>
+  </si>
+  <si>
+    <t>10.96.122.87</t>
+  </si>
+  <si>
+    <t>10.96.122.88</t>
+  </si>
+  <si>
+    <t>10.96.122.89</t>
+  </si>
+  <si>
+    <t>10.96.122.90</t>
+  </si>
+  <si>
+    <t>10.96.122.91</t>
+  </si>
+  <si>
+    <t>10.96.122.92</t>
+  </si>
+  <si>
+    <t>10.96.122.93</t>
+  </si>
+  <si>
+    <t>10.96.122.94</t>
+  </si>
+  <si>
+    <t>10.96.122.95</t>
+  </si>
+  <si>
+    <t>10.96.122.96</t>
+  </si>
+  <si>
+    <t>10.96.122.97</t>
+  </si>
+  <si>
+    <t>10.96.122.98</t>
+  </si>
+  <si>
+    <t>10.96.122.99</t>
+  </si>
+  <si>
+    <t>10.96.122.100</t>
+  </si>
+  <si>
+    <t>10.96.122.101</t>
+  </si>
+  <si>
+    <t>10.96.122.102</t>
+  </si>
+  <si>
+    <t>10.96.122.103</t>
+  </si>
+  <si>
+    <t>10.96.122.104</t>
+  </si>
+  <si>
+    <t>10.96.122.105</t>
+  </si>
+  <si>
+    <t>10.96.122.106</t>
+  </si>
+  <si>
+    <t>10.96.122.107</t>
+  </si>
+  <si>
+    <t>10.96.122.108</t>
+  </si>
+  <si>
+    <t>10.96.122.109</t>
+  </si>
+  <si>
+    <t>10.96.122.110</t>
+  </si>
+  <si>
+    <t>10.96.122.111</t>
+  </si>
+  <si>
+    <t>10.96.122.112</t>
+  </si>
+  <si>
+    <t>10.96.122.113</t>
+  </si>
+  <si>
+    <t>10.96.122.114</t>
+  </si>
+  <si>
+    <t>10.96.122.115</t>
+  </si>
+  <si>
+    <t>10.96.122.116</t>
+  </si>
+  <si>
+    <t>10.96.122.117</t>
+  </si>
+  <si>
+    <t>10.96.122.118</t>
+  </si>
+  <si>
+    <t>10.96.122.119</t>
+  </si>
+  <si>
+    <t>10.96.122.120</t>
+  </si>
+  <si>
+    <t>10.96.122.121</t>
+  </si>
+  <si>
+    <t>10.96.122.122</t>
+  </si>
+  <si>
+    <t>10.96.122.123</t>
+  </si>
+  <si>
+    <t>10.96.122.124</t>
+  </si>
+  <si>
+    <t>10.96.122.125</t>
+  </si>
+  <si>
+    <t>10.96.122.126</t>
+  </si>
+  <si>
+    <t>10.96.122.127</t>
+  </si>
+  <si>
+    <t>10.96.122.128</t>
+  </si>
+  <si>
+    <t>10.96.122.129</t>
+  </si>
+  <si>
+    <t>10.96.122.130</t>
+  </si>
+  <si>
+    <t>10.96.122.131</t>
+  </si>
+  <si>
+    <t>10.96.122.132</t>
+  </si>
+  <si>
+    <t>10.96.122.133</t>
+  </si>
+  <si>
+    <t>10.96.122.134</t>
+  </si>
+  <si>
+    <t>10.96.122.135</t>
+  </si>
+  <si>
+    <t>10.96.122.136</t>
+  </si>
+  <si>
+    <t>10.96.122.137</t>
+  </si>
+  <si>
+    <t>10.96.122.138</t>
+  </si>
+  <si>
+    <t>10.96.122.139</t>
+  </si>
+  <si>
+    <t>10.96.122.140</t>
+  </si>
+  <si>
+    <t>10.96.122.141</t>
+  </si>
+  <si>
+    <t>10.96.122.142</t>
+  </si>
+  <si>
+    <t>10.96.122.143</t>
+  </si>
+  <si>
+    <t>10.96.122.144</t>
+  </si>
+  <si>
+    <t>10.96.122.145</t>
+  </si>
+  <si>
+    <t>10.96.122.146</t>
+  </si>
+  <si>
+    <t>10.96.122.147</t>
+  </si>
+  <si>
+    <t>10.96.122.148</t>
+  </si>
+  <si>
+    <t>10.96.122.149</t>
+  </si>
+  <si>
+    <t>10.96.122.150</t>
+  </si>
+  <si>
+    <t>10.96.122.151</t>
+  </si>
+  <si>
+    <t>10.96.122.152</t>
+  </si>
+  <si>
+    <t>10.96.122.153</t>
+  </si>
+  <si>
+    <t>10.96.122.154</t>
+  </si>
+  <si>
+    <t>10.96.122.155</t>
+  </si>
+  <si>
+    <t>10.96.122.156</t>
+  </si>
+  <si>
+    <t>10.96.122.157</t>
+  </si>
+  <si>
+    <t>10.96.122.158</t>
+  </si>
+  <si>
+    <t>10.96.122.159</t>
+  </si>
+  <si>
+    <t>10.96.122.160</t>
+  </si>
+  <si>
+    <t>10.96.122.161</t>
+  </si>
+  <si>
+    <t>10.96.122.162</t>
+  </si>
+  <si>
+    <t>10.96.122.163</t>
+  </si>
+  <si>
+    <t>10.96.122.164</t>
+  </si>
+  <si>
+    <t>10.96.122.165</t>
+  </si>
+  <si>
+    <t>10.96.122.166</t>
+  </si>
+  <si>
+    <t>10.96.122.167</t>
+  </si>
+  <si>
+    <t>10.96.122.168</t>
+  </si>
+  <si>
+    <t>10.96.122.169</t>
+  </si>
+  <si>
+    <t>10.96.122.170</t>
+  </si>
+  <si>
+    <t>10.96.122.171</t>
+  </si>
+  <si>
+    <t>10.96.122.172</t>
+  </si>
+  <si>
+    <t>10.96.122.173</t>
+  </si>
+  <si>
+    <t>10.96.122.174</t>
+  </si>
+  <si>
+    <t>10.96.122.175</t>
+  </si>
+  <si>
+    <t>10.96.122.176</t>
+  </si>
+  <si>
+    <t>10.96.122.177</t>
+  </si>
+  <si>
+    <t>10.96.122.178</t>
+  </si>
+  <si>
+    <t>10.96.122.179</t>
+  </si>
+  <si>
+    <t>10.96.122.180</t>
+  </si>
+  <si>
+    <t>10.96.122.181</t>
+  </si>
+  <si>
+    <t>10.96.122.182</t>
+  </si>
+  <si>
+    <t>10.96.122.183</t>
+  </si>
+  <si>
+    <t>10.96.122.184</t>
+  </si>
+  <si>
+    <t>10.96.122.185</t>
+  </si>
+  <si>
+    <t>10.96.122.186</t>
+  </si>
+  <si>
+    <t>10.96.122.187</t>
+  </si>
+  <si>
+    <t>10.96.122.188</t>
+  </si>
+  <si>
+    <t>10.96.122.189</t>
+  </si>
+  <si>
+    <t>10.96.122.190</t>
+  </si>
+  <si>
+    <t>10.96.122.191</t>
+  </si>
+  <si>
+    <t>10.96.122.192</t>
+  </si>
+  <si>
+    <t>10.96.122.193</t>
+  </si>
+  <si>
+    <t>10.96.122.194</t>
+  </si>
+  <si>
+    <t>10.96.122.195</t>
+  </si>
+  <si>
+    <t>10.96.122.196</t>
+  </si>
+  <si>
+    <t>10.96.122.197</t>
+  </si>
+  <si>
+    <t>10.96.122.198</t>
+  </si>
+  <si>
+    <t>10.96.122.199</t>
+  </si>
+  <si>
+    <t>10.96.122.200</t>
+  </si>
+  <si>
+    <t>10.96.122.201</t>
+  </si>
+  <si>
+    <t>10.96.122.202</t>
+  </si>
+  <si>
+    <t>10.96.122.203</t>
+  </si>
+  <si>
+    <t>10.96.122.204</t>
+  </si>
+  <si>
+    <t>10.96.122.205</t>
+  </si>
+  <si>
+    <t>10.96.122.206</t>
+  </si>
+  <si>
+    <t>10.96.122.207</t>
+  </si>
+  <si>
+    <t>10.96.122.208</t>
+  </si>
+  <si>
+    <t>10.96.122.209</t>
+  </si>
+  <si>
+    <t>10.96.122.210</t>
+  </si>
+  <si>
+    <t>10.96.122.211</t>
+  </si>
+  <si>
+    <t>10.96.122.212</t>
+  </si>
+  <si>
+    <t>10.96.122.213</t>
+  </si>
+  <si>
+    <t>10.96.122.214</t>
+  </si>
+  <si>
+    <t>10.96.122.215</t>
+  </si>
+  <si>
+    <t>10.96.122.216</t>
+  </si>
+  <si>
+    <t>10.96.122.217</t>
+  </si>
+  <si>
+    <t>10.96.122.218</t>
+  </si>
+  <si>
+    <t>10.96.122.219</t>
+  </si>
+  <si>
+    <t>10.96.122.220</t>
+  </si>
+  <si>
+    <t>10.96.122.221</t>
+  </si>
+  <si>
+    <t>10.96.122.222</t>
+  </si>
+  <si>
+    <t>10.96.122.223</t>
+  </si>
+  <si>
+    <t>10.96.122.224</t>
+  </si>
+  <si>
+    <t>10.96.122.225</t>
+  </si>
+  <si>
+    <t>10.96.122.226</t>
+  </si>
+  <si>
+    <t>10.96.122.227</t>
+  </si>
+  <si>
+    <t>10.96.122.228</t>
+  </si>
+  <si>
+    <t>10.96.122.229</t>
+  </si>
+  <si>
+    <t>10.96.122.230</t>
+  </si>
+  <si>
+    <t>10.96.122.231</t>
+  </si>
+  <si>
+    <t>10.96.122.232</t>
+  </si>
+  <si>
+    <t>10.96.122.233</t>
+  </si>
+  <si>
+    <t>10.96.122.234</t>
+  </si>
+  <si>
+    <t>10.96.122.235</t>
+  </si>
+  <si>
+    <t>10.96.122.236</t>
+  </si>
+  <si>
+    <t>10.96.122.237</t>
+  </si>
+  <si>
+    <t>10.96.122.238</t>
+  </si>
+  <si>
+    <t>10.96.122.239</t>
+  </si>
+  <si>
+    <t>10.96.122.240</t>
+  </si>
+  <si>
+    <t>10.96.123.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.123.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.123.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.123.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.96.123.5</t>
+  </si>
+  <si>
+    <t>10.96.123.6</t>
+  </si>
+  <si>
+    <t>10.96.123.7</t>
+  </si>
+  <si>
+    <t>10.96.123.8</t>
+  </si>
+  <si>
+    <t>10.96.123.9</t>
+  </si>
+  <si>
+    <t>10.96.123.10</t>
+  </si>
+  <si>
+    <t>10.96.123.11</t>
+  </si>
+  <si>
+    <t>10.96.123.12</t>
+  </si>
+  <si>
+    <t>10.96.123.13</t>
+  </si>
+  <si>
+    <t>10.96.123.14</t>
+  </si>
+  <si>
+    <t>10.96.123.15</t>
+  </si>
+  <si>
+    <t>10.96.123.16</t>
+  </si>
+  <si>
+    <t>10.96.123.17</t>
+  </si>
+  <si>
+    <t>10.96.123.18</t>
+  </si>
+  <si>
+    <t>10.96.123.19</t>
+  </si>
+  <si>
+    <t>10.96.123.20</t>
+  </si>
+  <si>
+    <t>10.96.123.21</t>
+  </si>
+  <si>
+    <t>10.96.123.22</t>
+  </si>
+  <si>
+    <t>10.96.123.23</t>
+  </si>
+  <si>
+    <t>10.96.123.24</t>
+  </si>
+  <si>
+    <t>10.96.123.25</t>
+  </si>
+  <si>
+    <t>10.96.123.26</t>
+  </si>
+  <si>
+    <t>10.96.123.27</t>
+  </si>
+  <si>
+    <t>10.96.123.28</t>
+  </si>
+  <si>
+    <t>10.96.123.29</t>
+  </si>
+  <si>
+    <t>10.96.123.30</t>
+  </si>
+  <si>
+    <t>10.96.123.31</t>
+  </si>
+  <si>
+    <t>10.96.123.32</t>
+  </si>
+  <si>
+    <t>10.96.123.33</t>
+  </si>
+  <si>
+    <t>10.96.123.34</t>
+  </si>
+  <si>
+    <t>10.96.123.35</t>
+  </si>
+  <si>
+    <t>10.96.123.36</t>
+  </si>
+  <si>
+    <t>10.96.123.37</t>
+  </si>
+  <si>
+    <t>10.96.123.38</t>
+  </si>
+  <si>
+    <t>10.96.123.39</t>
+  </si>
+  <si>
+    <t>10.96.123.40</t>
+  </si>
+  <si>
+    <t>10.96.123.41</t>
+  </si>
+  <si>
+    <t>10.96.123.42</t>
+  </si>
+  <si>
+    <t>10.96.123.43</t>
+  </si>
+  <si>
+    <t>10.96.123.44</t>
+  </si>
+  <si>
+    <t>10.96.123.45</t>
+  </si>
+  <si>
+    <t>10.96.123.46</t>
+  </si>
+  <si>
+    <t>10.96.123.47</t>
+  </si>
+  <si>
+    <t>10.96.123.48</t>
+  </si>
+  <si>
+    <t>10.96.123.49</t>
+  </si>
+  <si>
+    <t>10.96.123.50</t>
+  </si>
+  <si>
+    <t>10.96.123.51</t>
+  </si>
+  <si>
+    <t>10.96.123.52</t>
+  </si>
+  <si>
+    <t>10.96.123.53</t>
+  </si>
+  <si>
+    <t>10.96.123.54</t>
+  </si>
+  <si>
+    <t>10.96.123.55</t>
+  </si>
+  <si>
+    <t>10.96.123.56</t>
+  </si>
+  <si>
+    <t>10.96.123.57</t>
+  </si>
+  <si>
+    <t>10.96.123.58</t>
+  </si>
+  <si>
+    <t>10.96.123.59</t>
+  </si>
+  <si>
+    <t>10.96.123.60</t>
+  </si>
+  <si>
+    <t>10.96.123.61</t>
+  </si>
+  <si>
+    <t>10.96.123.62</t>
+  </si>
+  <si>
+    <t>10.96.123.63</t>
+  </si>
+  <si>
+    <t>10.96.123.64</t>
+  </si>
+  <si>
+    <t>10.96.123.65</t>
+  </si>
+  <si>
+    <t>10.96.123.66</t>
+  </si>
+  <si>
+    <t>10.96.123.67</t>
+  </si>
+  <si>
+    <t>10.96.123.68</t>
+  </si>
+  <si>
+    <t>10.96.123.69</t>
+  </si>
+  <si>
+    <t>10.96.123.70</t>
+  </si>
+  <si>
+    <t>10.96.123.71</t>
+  </si>
+  <si>
+    <t>10.96.123.72</t>
+  </si>
+  <si>
+    <t>10.96.123.73</t>
+  </si>
+  <si>
+    <t>10.96.123.74</t>
+  </si>
+  <si>
+    <t>10.96.123.75</t>
+  </si>
+  <si>
+    <t>10.96.123.76</t>
+  </si>
+  <si>
+    <t>10.96.123.77</t>
+  </si>
+  <si>
+    <t>10.96.123.78</t>
+  </si>
+  <si>
+    <t>10.96.123.79</t>
+  </si>
+  <si>
+    <t>10.96.123.80</t>
+  </si>
+  <si>
+    <t>10.96.123.81</t>
+  </si>
+  <si>
+    <t>10.96.123.82</t>
+  </si>
+  <si>
+    <t>10.96.123.83</t>
+  </si>
+  <si>
+    <t>10.96.123.84</t>
+  </si>
+  <si>
+    <t>10.96.123.85</t>
+  </si>
+  <si>
+    <t>10.96.123.86</t>
+  </si>
+  <si>
+    <t>10.96.123.87</t>
+  </si>
+  <si>
+    <t>10.96.123.88</t>
+  </si>
+  <si>
+    <t>10.96.123.89</t>
+  </si>
+  <si>
+    <t>10.96.123.90</t>
+  </si>
+  <si>
+    <t>10.96.123.91</t>
+  </si>
+  <si>
+    <t>10.96.123.92</t>
+  </si>
+  <si>
+    <t>10.96.123.93</t>
+  </si>
+  <si>
+    <t>10.96.123.94</t>
+  </si>
+  <si>
+    <t>10.96.123.95</t>
+  </si>
+  <si>
+    <t>10.96.123.96</t>
+  </si>
+  <si>
+    <t>10.96.123.97</t>
+  </si>
+  <si>
+    <t>10.96.123.98</t>
+  </si>
+  <si>
+    <t>10.96.123.99</t>
+  </si>
+  <si>
+    <t>10.96.123.100</t>
+  </si>
+  <si>
+    <t>10.96.123.101</t>
+  </si>
+  <si>
+    <t>10.96.123.102</t>
+  </si>
+  <si>
+    <t>10.96.123.103</t>
+  </si>
+  <si>
+    <t>10.96.123.104</t>
+  </si>
+  <si>
+    <t>10.96.123.105</t>
+  </si>
+  <si>
+    <t>10.96.123.106</t>
+  </si>
+  <si>
+    <t>10.96.123.107</t>
+  </si>
+  <si>
+    <t>10.96.123.108</t>
+  </si>
+  <si>
+    <t>10.96.123.109</t>
+  </si>
+  <si>
+    <t>10.96.123.110</t>
+  </si>
+  <si>
+    <t>10.96.123.111</t>
+  </si>
+  <si>
+    <t>10.96.123.112</t>
+  </si>
+  <si>
+    <t>10.96.123.113</t>
+  </si>
+  <si>
+    <t>10.96.123.114</t>
+  </si>
+  <si>
+    <t>10.96.123.115</t>
+  </si>
+  <si>
+    <t>10.96.123.116</t>
+  </si>
+  <si>
+    <t>10.96.123.117</t>
+  </si>
+  <si>
+    <t>10.96.123.118</t>
+  </si>
+  <si>
+    <t>10.96.123.119</t>
+  </si>
+  <si>
+    <t>10.96.123.120</t>
+  </si>
+  <si>
+    <t>10.96.123.121</t>
+  </si>
+  <si>
+    <t>10.96.123.122</t>
+  </si>
+  <si>
+    <t>10.96.123.123</t>
+  </si>
+  <si>
+    <t>10.96.123.124</t>
+  </si>
+  <si>
+    <t>10.96.123.125</t>
+  </si>
+  <si>
+    <t>10.96.123.126</t>
+  </si>
+  <si>
+    <t>10.96.123.127</t>
+  </si>
+  <si>
+    <t>10.96.123.128</t>
+  </si>
+  <si>
+    <t>10.96.123.129</t>
+  </si>
+  <si>
+    <t>10.96.123.130</t>
+  </si>
+  <si>
+    <t>10.96.123.131</t>
+  </si>
+  <si>
+    <t>10.96.123.132</t>
+  </si>
+  <si>
+    <t>10.96.123.133</t>
+  </si>
+  <si>
+    <t>10.96.123.134</t>
+  </si>
+  <si>
+    <t>10.96.123.135</t>
+  </si>
+  <si>
+    <t>10.96.123.136</t>
+  </si>
+  <si>
+    <t>10.96.123.137</t>
+  </si>
+  <si>
+    <t>10.96.123.138</t>
+  </si>
+  <si>
+    <t>10.96.123.139</t>
+  </si>
+  <si>
+    <t>10.96.123.140</t>
+  </si>
+  <si>
+    <t>10.96.123.141</t>
+  </si>
+  <si>
+    <t>10.96.123.142</t>
+  </si>
+  <si>
+    <t>10.96.123.143</t>
+  </si>
+  <si>
+    <t>10.96.123.144</t>
+  </si>
+  <si>
+    <t>10.96.123.145</t>
+  </si>
+  <si>
+    <t>10.96.123.146</t>
+  </si>
+  <si>
+    <t>10.96.123.147</t>
+  </si>
+  <si>
+    <t>10.96.123.148</t>
+  </si>
+  <si>
+    <t>10.96.123.149</t>
+  </si>
+  <si>
+    <t>10.96.123.150</t>
+  </si>
+  <si>
+    <t>10.96.123.151</t>
+  </si>
+  <si>
+    <t>10.96.123.152</t>
+  </si>
+  <si>
+    <t>10.96.123.153</t>
+  </si>
+  <si>
+    <t>10.96.123.154</t>
+  </si>
+  <si>
+    <t>10.96.123.155</t>
+  </si>
+  <si>
+    <t>10.96.123.156</t>
+  </si>
+  <si>
+    <t>10.96.123.157</t>
+  </si>
+  <si>
+    <t>10.96.123.158</t>
+  </si>
+  <si>
+    <t>10.96.123.159</t>
+  </si>
+  <si>
+    <t>10.96.123.160</t>
+  </si>
+  <si>
+    <t>10.96.123.161</t>
+  </si>
+  <si>
+    <t>10.96.123.162</t>
+  </si>
+  <si>
+    <t>10.96.123.163</t>
+  </si>
+  <si>
+    <t>10.96.123.164</t>
+  </si>
+  <si>
+    <t>10.96.123.165</t>
+  </si>
+  <si>
+    <t>10.96.123.166</t>
+  </si>
+  <si>
+    <t>10.96.123.167</t>
+  </si>
+  <si>
+    <t>10.96.123.168</t>
+  </si>
+  <si>
+    <t>10.96.123.169</t>
+  </si>
+  <si>
+    <t>10.96.123.170</t>
+  </si>
+  <si>
+    <t>10.96.123.171</t>
+  </si>
+  <si>
+    <t>10.96.123.172</t>
+  </si>
+  <si>
+    <t>10.96.123.173</t>
+  </si>
+  <si>
+    <t>10.96.123.174</t>
+  </si>
+  <si>
+    <t>10.96.123.175</t>
+  </si>
+  <si>
+    <t>10.96.123.176</t>
+  </si>
+  <si>
+    <t>10.96.123.177</t>
+  </si>
+  <si>
+    <t>10.96.123.178</t>
+  </si>
+  <si>
+    <t>10.96.123.179</t>
+  </si>
+  <si>
+    <t>10.96.123.180</t>
+  </si>
+  <si>
+    <t>10.96.123.181</t>
+  </si>
+  <si>
+    <t>10.96.123.182</t>
+  </si>
+  <si>
+    <t>10.96.123.183</t>
+  </si>
+  <si>
+    <t>10.96.123.184</t>
+  </si>
+  <si>
+    <t>10.96.123.185</t>
+  </si>
+  <si>
+    <t>10.96.123.186</t>
+  </si>
+  <si>
+    <t>10.96.123.187</t>
+  </si>
+  <si>
+    <t>10.96.123.188</t>
+  </si>
+  <si>
+    <t>10.96.123.189</t>
+  </si>
+  <si>
+    <t>10.96.123.190</t>
+  </si>
+  <si>
+    <t>10.96.123.191</t>
+  </si>
+  <si>
+    <t>10.96.123.192</t>
+  </si>
+  <si>
+    <t>10.96.123.193</t>
+  </si>
+  <si>
+    <t>10.96.123.194</t>
+  </si>
+  <si>
+    <t>10.96.123.195</t>
+  </si>
+  <si>
+    <t>10.96.123.196</t>
+  </si>
+  <si>
+    <t>10.96.123.197</t>
+  </si>
+  <si>
+    <t>10.96.123.198</t>
+  </si>
+  <si>
+    <t>10.96.123.199</t>
+  </si>
+  <si>
+    <t>10.96.123.200</t>
+  </si>
+  <si>
+    <t>10.96.123.201</t>
+  </si>
+  <si>
+    <t>10.96.123.202</t>
+  </si>
+  <si>
+    <t>10.96.123.203</t>
+  </si>
+  <si>
+    <t>10.96.123.204</t>
+  </si>
+  <si>
+    <t>10.96.123.205</t>
+  </si>
+  <si>
+    <t>10.96.123.206</t>
+  </si>
+  <si>
+    <t>10.96.123.207</t>
+  </si>
+  <si>
+    <t>10.96.123.208</t>
+  </si>
+  <si>
+    <t>10.96.123.209</t>
+  </si>
+  <si>
+    <t>10.96.123.210</t>
+  </si>
+  <si>
+    <t>10.96.123.211</t>
+  </si>
+  <si>
+    <t>10.96.123.212</t>
+  </si>
+  <si>
+    <t>10.96.123.213</t>
+  </si>
+  <si>
+    <t>10.96.123.214</t>
+  </si>
+  <si>
+    <t>10.96.123.215</t>
+  </si>
+  <si>
+    <t>10.96.123.216</t>
+  </si>
+  <si>
+    <t>10.96.123.217</t>
+  </si>
+  <si>
+    <t>10.96.123.218</t>
+  </si>
+  <si>
+    <t>10.96.123.219</t>
+  </si>
+  <si>
+    <t>10.96.123.220</t>
+  </si>
+  <si>
+    <t>10.96.123.221</t>
+  </si>
+  <si>
+    <t>10.96.123.222</t>
+  </si>
+  <si>
+    <t>10.96.123.223</t>
+  </si>
+  <si>
+    <t>10.96.123.224</t>
+  </si>
+  <si>
+    <t>10.96.123.225</t>
+  </si>
+  <si>
+    <t>10.96.123.226</t>
+  </si>
+  <si>
+    <t>10.96.123.227</t>
+  </si>
+  <si>
+    <t>10.96.123.228</t>
+  </si>
+  <si>
+    <t>10.96.123.229</t>
+  </si>
+  <si>
+    <t>10.96.123.230</t>
+  </si>
+  <si>
+    <t>10.96.123.231</t>
+  </si>
+  <si>
+    <t>10.96.123.232</t>
+  </si>
+  <si>
+    <t>10.96.123.233</t>
+  </si>
+  <si>
+    <t>10.96.123.234</t>
+  </si>
+  <si>
+    <t>10.96.123.235</t>
+  </si>
+  <si>
+    <t>10.96.123.236</t>
+  </si>
+  <si>
+    <t>10.96.123.237</t>
+  </si>
+  <si>
+    <t>10.96.123.238</t>
+  </si>
+  <si>
+    <t>10.96.123.239</t>
+  </si>
+  <si>
+    <t>10.96.123.240</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="E349" sqref="E349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2407,6 +3855,2646 @@
         <v>237</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A121">
+        <v>2101</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A122">
+        <v>2102</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A123">
+        <v>2103</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A124">
+        <v>2104</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A125">
+        <v>2105</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A126">
+        <v>2106</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A127">
+        <v>2107</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A128">
+        <v>2108</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A129">
+        <v>2109</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A130">
+        <v>2110</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A131">
+        <v>2111</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A132">
+        <v>2112</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A133">
+        <v>2113</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A134">
+        <v>2114</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A135">
+        <v>2115</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A136">
+        <v>2116</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A137">
+        <v>2117</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A138">
+        <v>2118</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A139">
+        <v>2119</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A140">
+        <v>2120</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A141">
+        <v>2201</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A142">
+        <v>2202</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A143">
+        <v>2203</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A144">
+        <v>2204</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A145">
+        <v>2205</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A146">
+        <v>2206</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A147">
+        <v>2207</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A148">
+        <v>2208</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A149">
+        <v>2209</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A150">
+        <v>2210</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A151">
+        <v>2211</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A152">
+        <v>2212</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A153">
+        <v>2213</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A154">
+        <v>2214</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A155">
+        <v>2215</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A156">
+        <v>2216</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A157">
+        <v>2217</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A158">
+        <v>2218</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A159">
+        <v>2219</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A160">
+        <v>2220</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A161">
+        <v>2301</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A162">
+        <v>2302</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A163">
+        <v>2303</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A164">
+        <v>2304</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A165">
+        <v>2305</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A166">
+        <v>2306</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A167">
+        <v>2307</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A168">
+        <v>2308</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A169">
+        <v>2309</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A170">
+        <v>2310</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A171">
+        <v>2311</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A172">
+        <v>2312</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A173">
+        <v>2313</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A174">
+        <v>2314</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A175">
+        <v>2315</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A176">
+        <v>2316</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A177">
+        <v>2317</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A178">
+        <v>2318</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A179">
+        <v>2319</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A180">
+        <v>2320</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A181">
+        <v>2401</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A182">
+        <v>2402</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A183">
+        <v>2403</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A184">
+        <v>2404</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A185">
+        <v>2405</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A186">
+        <v>2406</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A187">
+        <v>2407</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A188">
+        <v>2408</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A189">
+        <v>2409</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A190">
+        <v>2410</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A191">
+        <v>2411</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A192">
+        <v>2412</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A193">
+        <v>2413</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A194">
+        <v>2414</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A195">
+        <v>2415</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A196">
+        <v>2416</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A197">
+        <v>2417</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A198">
+        <v>2418</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A199">
+        <v>2419</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A200">
+        <v>2420</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A201">
+        <v>2501</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A202">
+        <v>2502</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A203">
+        <v>2503</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A204">
+        <v>2504</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A205">
+        <v>2505</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A206">
+        <v>2506</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A207">
+        <v>2507</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A208">
+        <v>2508</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A209">
+        <v>2509</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A210">
+        <v>2510</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A211">
+        <v>2511</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A212">
+        <v>2512</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A213">
+        <v>2513</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A214">
+        <v>2514</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A215">
+        <v>2515</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A216">
+        <v>2516</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A217">
+        <v>2517</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A218">
+        <v>2518</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A219">
+        <v>2519</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A220">
+        <v>2520</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A221">
+        <v>2601</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A222">
+        <v>2602</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A223">
+        <v>2603</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A224">
+        <v>2604</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A225">
+        <v>2605</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A226">
+        <v>2606</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A227">
+        <v>2607</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A228">
+        <v>2608</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A229">
+        <v>2609</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A230">
+        <v>2610</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A231">
+        <v>2611</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A232">
+        <v>2612</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A233">
+        <v>2613</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A234">
+        <v>2614</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A235">
+        <v>2615</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A236">
+        <v>2616</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A237">
+        <v>2617</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A238">
+        <v>2618</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A239">
+        <v>2619</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A240">
+        <v>2620</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A241">
+        <v>3101</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A242">
+        <v>3102</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A243">
+        <v>3103</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A244">
+        <v>3104</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A245">
+        <v>3105</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A246">
+        <v>3106</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A247">
+        <v>3107</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A248">
+        <v>3108</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A249">
+        <v>3109</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A250">
+        <v>3110</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A251">
+        <v>3111</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A252">
+        <v>3112</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A253">
+        <v>3113</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A254">
+        <v>3114</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A255">
+        <v>3115</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A256">
+        <v>3116</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A257">
+        <v>3117</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A258">
+        <v>3118</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A259">
+        <v>3119</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A260">
+        <v>3120</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A261">
+        <v>3201</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A262">
+        <v>3202</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A263">
+        <v>3203</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A264">
+        <v>3204</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A265">
+        <v>3205</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A266">
+        <v>3206</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A267">
+        <v>3207</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A268">
+        <v>3208</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A269">
+        <v>3209</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A270">
+        <v>3210</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A271">
+        <v>3211</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A272">
+        <v>3212</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A273">
+        <v>3213</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A274">
+        <v>3214</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A275">
+        <v>3215</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A276">
+        <v>3216</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A277">
+        <v>3217</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A278">
+        <v>3218</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A279">
+        <v>3219</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A280">
+        <v>3220</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A281">
+        <v>3301</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A282">
+        <v>3302</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A283">
+        <v>3303</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A284">
+        <v>3304</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A285">
+        <v>3305</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A286">
+        <v>3306</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A287">
+        <v>3307</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A288">
+        <v>3308</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A289">
+        <v>3309</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A290">
+        <v>3310</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A291">
+        <v>3311</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A292">
+        <v>3312</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A293">
+        <v>3313</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A294">
+        <v>3314</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A295">
+        <v>3315</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A296">
+        <v>3316</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A297">
+        <v>3317</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A298">
+        <v>3318</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A299">
+        <v>3319</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A300">
+        <v>3320</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A301">
+        <v>3401</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A302">
+        <v>3402</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A303">
+        <v>3403</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A304">
+        <v>3404</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A305">
+        <v>3405</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A306">
+        <v>3406</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A307">
+        <v>3407</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A308">
+        <v>3408</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A309">
+        <v>3409</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A310">
+        <v>3410</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A311">
+        <v>3411</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A312">
+        <v>3412</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A313">
+        <v>3413</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A314">
+        <v>3414</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A315">
+        <v>3415</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A316">
+        <v>3416</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A317">
+        <v>3417</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A318">
+        <v>3418</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A319">
+        <v>3419</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A320">
+        <v>3420</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A321">
+        <v>3501</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A322">
+        <v>3502</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A323">
+        <v>3503</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A324">
+        <v>3504</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A325">
+        <v>3505</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A326">
+        <v>3506</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A327">
+        <v>3507</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A328">
+        <v>3508</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A329">
+        <v>3509</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A330">
+        <v>3510</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A331">
+        <v>3511</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A332">
+        <v>3512</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A333">
+        <v>3513</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A334">
+        <v>3514</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A335">
+        <v>3515</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A336">
+        <v>3516</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A337">
+        <v>3517</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A338">
+        <v>3518</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A339">
+        <v>3519</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A340">
+        <v>3520</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A341">
+        <v>3601</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A342">
+        <v>3602</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A343">
+        <v>3603</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A344">
+        <v>3604</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A345">
+        <v>3605</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A346">
+        <v>3606</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A347">
+        <v>3607</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A348">
+        <v>3608</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A349">
+        <v>3609</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A350">
+        <v>3610</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A351">
+        <v>3611</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A352">
+        <v>3612</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A353">
+        <v>3613</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A354">
+        <v>3614</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A355">
+        <v>3615</v>
+      </c>
+      <c r="B355" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A356">
+        <v>3616</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A357">
+        <v>3617</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A358">
+        <v>3618</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A359">
+        <v>3619</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A360">
+        <v>3620</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>